<commit_message>
1 camada 15 neu
</commit_message>
<xml_diff>
--- a/nuno-dataset/test-oxigen-01/content/results/metrics_11_7.xlsx
+++ b/nuno-dataset/test-oxigen-01/content/results/metrics_11_7.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,776 +478,559 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_0</t>
+          <t>model_11_7_17</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7966347679529389</v>
+        <v>0.7002516648192787</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7474099282913303</v>
+        <v>0.3647322835975876</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8345691892655929</v>
+        <v>-0.07994281125102876</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8089050122182183</v>
+        <v>0.1709557656501347</v>
       </c>
       <c r="F2" t="n">
-        <v>0.2250653803348541</v>
+        <v>0.3317330479621887</v>
       </c>
       <c r="G2" t="n">
-        <v>0.2321533560752869</v>
+        <v>0.8481671214103699</v>
       </c>
       <c r="H2" t="n">
-        <v>0.2896773517131805</v>
+        <v>1.255890846252441</v>
       </c>
       <c r="I2" t="n">
-        <v>0.259223610162735</v>
+        <v>1.04003632068634</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_1</t>
+          <t>model_11_7_10</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7967597142025742</v>
+        <v>0.7079067264287653</v>
       </c>
       <c r="C3" t="n">
-        <v>0.7263258660707106</v>
+        <v>0.4813885791713711</v>
       </c>
       <c r="D3" t="n">
-        <v>0.7977922060519287</v>
+        <v>-0.1419645515159547</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7790018273334031</v>
+        <v>0.2096286272787826</v>
       </c>
       <c r="F3" t="n">
-        <v>0.2249270975589752</v>
+        <v>0.3232612013816833</v>
       </c>
       <c r="G3" t="n">
-        <v>0.2515315413475037</v>
+        <v>0.6924154162406921</v>
       </c>
       <c r="H3" t="n">
-        <v>0.3540756106376648</v>
+        <v>1.328017354011536</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2997877597808838</v>
+        <v>0.9915212988853455</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_2</t>
+          <t>model_11_7_16</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8426870902841885</v>
+        <v>0.7084634804740617</v>
       </c>
       <c r="C4" t="n">
-        <v>0.7457845256345799</v>
+        <v>0.3721049167583707</v>
       </c>
       <c r="D4" t="n">
-        <v>0.7946766731441101</v>
+        <v>-0.03201855918362462</v>
       </c>
       <c r="E4" t="n">
-        <v>0.784089076577582</v>
+        <v>0.1960160232365913</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1740990430116653</v>
+        <v>0.3226450085639954</v>
       </c>
       <c r="G4" t="n">
-        <v>0.2336472719907761</v>
+        <v>0.8383236527442932</v>
       </c>
       <c r="H4" t="n">
-        <v>0.3595310747623444</v>
+        <v>1.200158596038818</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2928868532180786</v>
+        <v>1.008598208427429</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_3</t>
+          <t>model_11_7_9</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.8456253215260898</v>
+        <v>0.712576180391746</v>
       </c>
       <c r="C5" t="n">
-        <v>0.6519253734808472</v>
+        <v>0.5100393095531759</v>
       </c>
       <c r="D5" t="n">
-        <v>0.7428676713240323</v>
+        <v>-0.1233196162426005</v>
       </c>
       <c r="E5" t="n">
-        <v>0.7189505898418798</v>
+        <v>0.2339032846595611</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1708472818136215</v>
+        <v>0.3180935084819794</v>
       </c>
       <c r="G5" t="n">
-        <v>0.3199124038219452</v>
+        <v>0.6541628837585449</v>
       </c>
       <c r="H5" t="n">
-        <v>0.4502511322498322</v>
+        <v>1.306334733963013</v>
       </c>
       <c r="I5" t="n">
-        <v>0.381248265504837</v>
+        <v>0.9610686302185059</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_6</t>
+          <t>model_11_7_8</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8575958073999357</v>
+        <v>0.7181493871138978</v>
       </c>
       <c r="C6" t="n">
-        <v>0.4835238362263473</v>
+        <v>0.5488765729452487</v>
       </c>
       <c r="D6" t="n">
-        <v>0.7728658414248526</v>
+        <v>-0.1153302558281311</v>
       </c>
       <c r="E6" t="n">
-        <v>0.6767680628764672</v>
+        <v>0.2592713462343698</v>
       </c>
       <c r="F6" t="n">
-        <v>0.1575994789600372</v>
+        <v>0.3119255602359772</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4746887981891632</v>
+        <v>0.6023099422454834</v>
       </c>
       <c r="H6" t="n">
-        <v>0.3977228999137878</v>
+        <v>1.297043681144714</v>
       </c>
       <c r="I6" t="n">
-        <v>0.4384695887565613</v>
+        <v>0.929244339466095</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_5</t>
+          <t>model_11_7_15</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8635683076005556</v>
+        <v>0.7226953047667299</v>
       </c>
       <c r="C7" t="n">
-        <v>0.524093185765817</v>
+        <v>0.4445007811534527</v>
       </c>
       <c r="D7" t="n">
-        <v>0.7860395481998873</v>
+        <v>-0.02712678258419787</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6993225571069787</v>
+        <v>0.2389407993394956</v>
       </c>
       <c r="F7" t="n">
-        <v>0.1509896665811539</v>
+        <v>0.3068945705890656</v>
       </c>
       <c r="G7" t="n">
-        <v>0.4374018311500549</v>
+        <v>0.7416656017303467</v>
       </c>
       <c r="H7" t="n">
-        <v>0.3746551275253296</v>
+        <v>1.194469809532166</v>
       </c>
       <c r="I7" t="n">
-        <v>0.4078740477561951</v>
+        <v>0.9547489285469055</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_7</t>
+          <t>model_11_7_12</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.8642120299493354</v>
+        <v>0.7301507214222664</v>
       </c>
       <c r="C8" t="n">
-        <v>0.5053230459178182</v>
+        <v>0.4755559585346225</v>
       </c>
       <c r="D8" t="n">
-        <v>0.7497157262744438</v>
+        <v>-0.0010107709658147</v>
       </c>
       <c r="E8" t="n">
-        <v>0.6705247772650591</v>
+        <v>0.2678304753926649</v>
       </c>
       <c r="F8" t="n">
-        <v>0.1502772718667984</v>
+        <v>0.2986436188220978</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4546533226966858</v>
+        <v>0.7002027034759521</v>
       </c>
       <c r="H8" t="n">
-        <v>0.4382598698139191</v>
+        <v>1.164098858833313</v>
       </c>
       <c r="I8" t="n">
-        <v>0.446938693523407</v>
+        <v>0.9185069799423218</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_9</t>
+          <t>model_11_7_11</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.8736056109600707</v>
+        <v>0.7305844059180946</v>
       </c>
       <c r="C9" t="n">
-        <v>0.552584279872963</v>
+        <v>0.4941880252414723</v>
       </c>
       <c r="D9" t="n">
-        <v>0.7434632729244132</v>
+        <v>-0.01702995621902148</v>
       </c>
       <c r="E9" t="n">
-        <v>0.6836789584489598</v>
+        <v>0.2713408727243324</v>
       </c>
       <c r="F9" t="n">
-        <v>0.139881357550621</v>
+        <v>0.2981636822223663</v>
       </c>
       <c r="G9" t="n">
-        <v>0.4112159311771393</v>
+        <v>0.6753264665603638</v>
       </c>
       <c r="H9" t="n">
-        <v>0.4492082297801971</v>
+        <v>1.182727932929993</v>
       </c>
       <c r="I9" t="n">
-        <v>0.4290948212146759</v>
+        <v>0.9141031503677368</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_4</t>
+          <t>model_11_7_7</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.8748538016856184</v>
+        <v>0.7327311461080099</v>
       </c>
       <c r="C10" t="n">
-        <v>0.6804490245356662</v>
+        <v>0.5842233517790264</v>
       </c>
       <c r="D10" t="n">
-        <v>0.788668464025571</v>
+        <v>-0.02075334710451893</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7570037872531364</v>
+        <v>0.3204458409667452</v>
       </c>
       <c r="F10" t="n">
-        <v>0.1384999603033066</v>
+        <v>0.2957878708839417</v>
       </c>
       <c r="G10" t="n">
-        <v>0.2936965525150299</v>
+        <v>0.5551173090934753</v>
       </c>
       <c r="H10" t="n">
-        <v>0.3700517416000366</v>
+        <v>1.187057971954346</v>
       </c>
       <c r="I10" t="n">
-        <v>0.3296284675598145</v>
+        <v>0.8525009751319885</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_8</t>
+          <t>model_11_7_14</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.8781199381435385</v>
+        <v>0.7339764847055407</v>
       </c>
       <c r="C11" t="n">
-        <v>0.5741966682723262</v>
+        <v>0.4823647614386469</v>
       </c>
       <c r="D11" t="n">
-        <v>0.7539712916598075</v>
+        <v>0.003591012351457756</v>
       </c>
       <c r="E11" t="n">
-        <v>0.6978145274552471</v>
+        <v>0.2736738508886775</v>
       </c>
       <c r="F11" t="n">
-        <v>0.134885311126709</v>
+        <v>0.2944096922874451</v>
       </c>
       <c r="G11" t="n">
-        <v>0.3913521468639374</v>
+        <v>0.6911121010780334</v>
       </c>
       <c r="H11" t="n">
-        <v>0.4308081865310669</v>
+        <v>1.158747315406799</v>
       </c>
       <c r="I11" t="n">
-        <v>0.4099196791648865</v>
+        <v>0.9111764430999756</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_18</t>
+          <t>model_11_7_3</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.8795910111717798</v>
+        <v>0.7370067779662957</v>
       </c>
       <c r="C12" t="n">
-        <v>0.6820247075635075</v>
+        <v>0.650091287612325</v>
       </c>
       <c r="D12" t="n">
-        <v>0.6796760784457425</v>
+        <v>-0.01194888856282095</v>
       </c>
       <c r="E12" t="n">
-        <v>0.6913612064670654</v>
+        <v>0.361399182532369</v>
       </c>
       <c r="F12" t="n">
-        <v>0.133257269859314</v>
+        <v>0.2910560071468353</v>
       </c>
       <c r="G12" t="n">
-        <v>0.2922483682632446</v>
+        <v>0.4671747982501984</v>
       </c>
       <c r="H12" t="n">
-        <v>0.5609027147293091</v>
+        <v>1.176819086074829</v>
       </c>
       <c r="I12" t="n">
-        <v>0.4186737537384033</v>
+        <v>0.8011249899864197</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_16</t>
+          <t>model_11_7_13</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.8798175814241737</v>
+        <v>0.7381709319140424</v>
       </c>
       <c r="C13" t="n">
-        <v>0.6545769435998776</v>
+        <v>0.4815306063831233</v>
       </c>
       <c r="D13" t="n">
-        <v>0.6987281537050498</v>
+        <v>0.03742744271572807</v>
       </c>
       <c r="E13" t="n">
-        <v>0.6930888029806158</v>
+        <v>0.2879664045012489</v>
       </c>
       <c r="F13" t="n">
-        <v>0.1330065280199051</v>
+        <v>0.2897676527500153</v>
       </c>
       <c r="G13" t="n">
-        <v>0.3174754083156586</v>
+        <v>0.6922258138656616</v>
       </c>
       <c r="H13" t="n">
-        <v>0.5275415778160095</v>
+        <v>1.11939811706543</v>
       </c>
       <c r="I13" t="n">
-        <v>0.4163302481174469</v>
+        <v>0.8932464122772217</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_12</t>
+          <t>model_11_7_2</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.880149559376336</v>
+        <v>0.7395940477339442</v>
       </c>
       <c r="C14" t="n">
-        <v>0.6100507372185351</v>
+        <v>0.6903707282720486</v>
       </c>
       <c r="D14" t="n">
-        <v>0.7324735531797149</v>
+        <v>0.04118575533857938</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6976162797410517</v>
+        <v>0.4072740668341531</v>
       </c>
       <c r="F14" t="n">
-        <v>0.1326391249895096</v>
+        <v>0.2881926596164703</v>
       </c>
       <c r="G14" t="n">
-        <v>0.3583990037441254</v>
+        <v>0.4133963584899902</v>
       </c>
       <c r="H14" t="n">
-        <v>0.4684517383575439</v>
+        <v>1.115027546882629</v>
       </c>
       <c r="I14" t="n">
-        <v>0.410188615322113</v>
+        <v>0.7435749173164368</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_10</t>
+          <t>model_11_7_5</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.880161328376899</v>
+        <v>0.7451315786145301</v>
       </c>
       <c r="C15" t="n">
-        <v>0.5962665483115165</v>
+        <v>0.6612800239998509</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7416541933992232</v>
+        <v>0.02486057436655531</v>
       </c>
       <c r="E15" t="n">
-        <v>0.6982489006230654</v>
+        <v>0.3837621685437096</v>
       </c>
       <c r="F15" t="n">
-        <v>0.1326261013746262</v>
+        <v>0.2820642590522766</v>
       </c>
       <c r="G15" t="n">
-        <v>0.3710679411888123</v>
+        <v>0.4522363245487213</v>
       </c>
       <c r="H15" t="n">
-        <v>0.4523759782314301</v>
+        <v>1.134012460708618</v>
       </c>
       <c r="I15" t="n">
-        <v>0.4093304574489594</v>
+        <v>0.7730706334114075</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_17</t>
+          <t>model_11_7_1</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.8804235842986881</v>
+        <v>0.750985144586181</v>
       </c>
       <c r="C16" t="n">
-        <v>0.6633410588096069</v>
+        <v>0.7398652179400935</v>
       </c>
       <c r="D16" t="n">
-        <v>0.6953166661456267</v>
+        <v>0.1380216109653867</v>
       </c>
       <c r="E16" t="n">
-        <v>0.6941602336007682</v>
+        <v>0.4774032061269813</v>
       </c>
       <c r="F16" t="n">
-        <v>0.1323358565568924</v>
+        <v>0.2755860686302185</v>
       </c>
       <c r="G16" t="n">
-        <v>0.3094203472137451</v>
+        <v>0.3473146259784698</v>
       </c>
       <c r="H16" t="n">
-        <v>0.5335152149200439</v>
+        <v>1.00241494178772</v>
       </c>
       <c r="I16" t="n">
-        <v>0.4148768186569214</v>
+        <v>0.6555978655815125</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_15</t>
+          <t>model_11_7_0</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.8806907031397042</v>
+        <v>0.7528091550918616</v>
       </c>
       <c r="C17" t="n">
-        <v>0.6500343316419908</v>
+        <v>0.7363294929098292</v>
       </c>
       <c r="D17" t="n">
-        <v>0.7061029691536334</v>
+        <v>0.1577917688373283</v>
       </c>
       <c r="E17" t="n">
-        <v>0.6959393154210708</v>
+        <v>0.4840367512708251</v>
       </c>
       <c r="F17" t="n">
-        <v>0.1320402473211288</v>
+        <v>0.2735674381256104</v>
       </c>
       <c r="G17" t="n">
-        <v>0.3216504156589508</v>
+        <v>0.3520352840423584</v>
       </c>
       <c r="H17" t="n">
-        <v>0.5146279335021973</v>
+        <v>0.9794236421585083</v>
       </c>
       <c r="I17" t="n">
-        <v>0.4124634265899658</v>
+        <v>0.6472761631011963</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_14</t>
+          <t>model_11_7_4</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.8811166051212574</v>
+        <v>0.757896496948585</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6365873006952287</v>
+        <v>0.6746880336809581</v>
       </c>
       <c r="D18" t="n">
-        <v>0.7173773734558653</v>
+        <v>0.09286371297776708</v>
       </c>
       <c r="E18" t="n">
-        <v>0.6979645219343109</v>
+        <v>0.4209801886542373</v>
       </c>
       <c r="F18" t="n">
-        <v>0.1315688937902451</v>
+        <v>0.2679372429847717</v>
       </c>
       <c r="G18" t="n">
-        <v>0.3340094983577728</v>
+        <v>0.4343348741531372</v>
       </c>
       <c r="H18" t="n">
-        <v>0.4948858618736267</v>
+        <v>1.054929971694946</v>
       </c>
       <c r="I18" t="n">
-        <v>0.4097162783145905</v>
+        <v>0.7263805866241455</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>model_11_7_22</t>
+          <t>model_11_7_6</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.8814348435498062</v>
+        <v>0.762659470107363</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6965245635792112</v>
+        <v>0.655460316102721</v>
       </c>
       <c r="D19" t="n">
-        <v>0.6773456029972659</v>
+        <v>0.1084628072773595</v>
       </c>
       <c r="E19" t="n">
-        <v>0.6951464490839816</v>
+        <v>0.4169504137038907</v>
       </c>
       <c r="F19" t="n">
-        <v>0.1312166899442673</v>
+        <v>0.2626660168170929</v>
       </c>
       <c r="G19" t="n">
-        <v>0.2789216637611389</v>
+        <v>0.4600063860416412</v>
       </c>
       <c r="H19" t="n">
-        <v>0.5649834871292114</v>
+        <v>1.036789417266846</v>
       </c>
       <c r="I19" t="n">
-        <v>0.4135389924049377</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>model_11_7_21</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>0.8815105504108602</v>
-      </c>
-      <c r="C20" t="n">
-        <v>0.6960289134592071</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0.6779927454840726</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.6953617599667217</v>
-      </c>
-      <c r="F20" t="n">
-        <v>0.1311329156160355</v>
-      </c>
-      <c r="G20" t="n">
-        <v>0.2793772220611572</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0.5638502836227417</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0.4132468700408936</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>model_11_7_20</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>0.8820920232116406</v>
-      </c>
-      <c r="C21" t="n">
-        <v>0.6971468118909592</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0.6802139019783551</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.6971120237073201</v>
-      </c>
-      <c r="F21" t="n">
-        <v>0.1304893791675568</v>
-      </c>
-      <c r="G21" t="n">
-        <v>0.278349757194519</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.5599609613418579</v>
-      </c>
-      <c r="I21" t="n">
-        <v>0.4108726978302002</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>model_11_7_19</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>0.8821947514858487</v>
-      </c>
-      <c r="C22" t="n">
-        <v>0.6960948137762568</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0.6815349330863278</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0.6975372097772359</v>
-      </c>
-      <c r="F22" t="n">
-        <v>0.1303756982088089</v>
-      </c>
-      <c r="G22" t="n">
-        <v>0.279316633939743</v>
-      </c>
-      <c r="H22" t="n">
-        <v>0.557647705078125</v>
-      </c>
-      <c r="I22" t="n">
-        <v>0.4102958738803864</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>model_11_7_13</t>
-        </is>
-      </c>
-      <c r="B23" t="n">
-        <v>0.8823510193826426</v>
-      </c>
-      <c r="C23" t="n">
-        <v>0.6281817402247921</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0.729406887557976</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0.7022569553422655</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.1302027553319931</v>
-      </c>
-      <c r="G23" t="n">
-        <v>0.3417349755764008</v>
-      </c>
-      <c r="H23" t="n">
-        <v>0.4738216400146484</v>
-      </c>
-      <c r="I23" t="n">
-        <v>0.4038935005664825</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>model_11_7_11</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>0.8823748165537588</v>
-      </c>
-      <c r="C24" t="n">
-        <v>0.6166632028143677</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.7391131852020238</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0.7040213950720653</v>
-      </c>
-      <c r="F24" t="n">
-        <v>0.1301764100790024</v>
-      </c>
-      <c r="G24" t="n">
-        <v>0.3523215353488922</v>
-      </c>
-      <c r="H24" t="n">
-        <v>0.4568254351615906</v>
-      </c>
-      <c r="I24" t="n">
-        <v>0.4014999568462372</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>model_11_7_23</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>0.8826207423081108</v>
-      </c>
-      <c r="C25" t="n">
-        <v>0.7024464240275469</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0.6789199623434825</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0.698226976070498</v>
-      </c>
-      <c r="F25" t="n">
-        <v>0.1299042552709579</v>
-      </c>
-      <c r="G25" t="n">
-        <v>0.2734789252281189</v>
-      </c>
-      <c r="H25" t="n">
-        <v>0.5622266530990601</v>
-      </c>
-      <c r="I25" t="n">
-        <v>0.4093602001667023</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>model_11_7_24</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>0.8829811167221238</v>
-      </c>
-      <c r="C26" t="n">
-        <v>0.707367872726101</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0.6773480439533712</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.6990373690302865</v>
-      </c>
-      <c r="F26" t="n">
-        <v>0.1295054107904434</v>
-      </c>
-      <c r="G26" t="n">
-        <v>0.2689556479454041</v>
-      </c>
-      <c r="H26" t="n">
-        <v>0.5649791955947876</v>
-      </c>
-      <c r="I26" t="n">
-        <v>0.4082609117031097</v>
+        <v>0.7314359545707703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>